<commit_message>
figures, run, fix remaining inconsistencies
</commit_message>
<xml_diff>
--- a/data/poverty/WID_income.xlsx
+++ b/data/poverty/WID_income.xlsx
@@ -920,7 +920,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="G13" s="1">
         <f>100*E14/(E13-C13)</f>
-        <v>3.5204940656914159E-2</v>
+        <v>3.5393194991594108E-2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1182,11 +1182,11 @@
         <v>18</v>
       </c>
       <c r="E14">
-        <v>112.2418</v>
+        <v>112.842</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>9.3534833333333331</v>
+        <v>9.4034999999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>